<commit_message>
Creating the analyses R analytic code
</commit_message>
<xml_diff>
--- a/Myanmar Project_Code Book.xlsx
+++ b/Myanmar Project_Code Book.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phyllislun/Documents/GitHub/Myanmar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phyllislun/Documents/GitHub/myanmar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B73ED3-CC73-C54D-8BB7-F9BF92B8F8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C17E648-3CF0-074E-93AD-745C7E8E4400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="740" windowWidth="18520" windowHeight="18380" xr2:uid="{38EF2D11-A97C-5F49-8E7A-12D4A1CCF98A}"/>
+    <workbookView xWindow="35300" yWindow="-360" windowWidth="28500" windowHeight="18380" xr2:uid="{38EF2D11-A97C-5F49-8E7A-12D4A1CCF98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$52</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
   <si>
     <t>Category</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Do you approve or disapprove of the job performance of the leadership of this country?</t>
-  </si>
-  <si>
-    <t>WP112</t>
   </si>
   <si>
     <t>WP137</t>
@@ -241,12 +238,6 @@
     <t>In this country, do you have confidence in each of the following, or not? How about the military?</t>
   </si>
   <si>
-    <t>Confidence in local police force</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In the city or area where you live, do you have confidence in the local police force, or not?</t>
-  </si>
-  <si>
     <t>Prosocial</t>
   </si>
   <si>
@@ -288,9 +279,6 @@
     <t>Have you done any of the following in the past month? How about helped a stranger or someone you didn't know who needed help?</t>
   </si>
   <si>
-    <t>WP111</t>
-  </si>
-  <si>
     <t>WP1325</t>
   </si>
   <si>
@@ -303,31 +291,16 @@
     <t xml:space="preserve"> Ideally, if you had the opportunity, would you like to move PERMANENTLY to another country, or would you prefer to continue living in this country?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Have you done any of the following in the past month? How about voiced your opinion to a public official?</t>
-  </si>
-  <si>
-    <t>Voicing opinion to public official</t>
-  </si>
-  <si>
     <t>Intention to move to another country</t>
   </si>
   <si>
     <t>Satisifaction with freedom to choose</t>
   </si>
   <si>
-    <t>Minorities</t>
-  </si>
-  <si>
     <t>WP103</t>
   </si>
   <si>
     <t>Is the city or area where you live a good place or not a good place to live for racial and ethnic minorities?</t>
-  </si>
-  <si>
-    <t>Minority friendly</t>
-  </si>
-  <si>
-    <t>Freedom of Media</t>
   </si>
   <si>
     <t>WP10251</t>
@@ -628,6 +601,12 @@
   </si>
   <si>
     <t>Civil society</t>
+  </si>
+  <si>
+    <t>racial/ ethnic minorities</t>
+  </si>
+  <si>
+    <t>freedom of media</t>
   </si>
 </sst>
 </file>
@@ -699,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -717,24 +696,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1064,10 +1053,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EAD5B6-1AAF-194F-84E0-06751B52E2D1}">
-  <dimension ref="A1:G54"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C54"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1104,75 +1094,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="E3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>151</v>
+      </c>
+      <c r="E5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1180,16 +1167,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1197,185 +1184,181 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="D13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="8" t="s">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="F15" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" t="s">
-        <v>173</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>137</v>
+      <c r="F16" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -1383,19 +1366,19 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>94</v>
+        <v>67</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -1403,19 +1386,19 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>97</v>
+        <v>68</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -1423,39 +1406,39 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1463,99 +1446,90 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1563,60 +1537,61 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>147</v>
+        <v>165</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>167</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>174</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>134</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28"/>
     </row>
     <row r="29" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1626,19 +1601,19 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1646,18 +1621,17 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>175</v>
+        <v>59</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G30"/>
+        <v>126</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1667,39 +1641,36 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1707,198 +1678,193 @@
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>166</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="D34" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="D35" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" ht="237" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:7" ht="237" customHeight="1" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>133</v>
+        <v>88</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1906,135 +1872,156 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>130</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>131</v>
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
-      </c>
-      <c r="E47" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>18</v>
       </c>
       <c r="D48" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>160</v>
-      </c>
-      <c r="E49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
-      </c>
-      <c r="E50" t="s">
-        <v>129</v>
+        <v>36</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2042,78 +2029,51 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="C51" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>37</v>
       </c>
       <c r="E51" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
+        <v>38</v>
       </c>
       <c r="E52" t="s">
-        <v>127</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" t="s">
-        <v>120</v>
-      </c>
-      <c r="D53" t="s">
-        <v>121</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D54" t="s">
-        <v>124</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G54" xr:uid="{D9EAD5B6-1AAF-194F-84E0-06751B52E2D1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G54">
-      <sortCondition ref="B1:B54"/>
+  <autoFilter ref="A1:G52" xr:uid="{D9EAD5B6-1AAF-194F-84E0-06751B52E2D1}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Gallup World Poll"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G52">
+      <sortCondition ref="C1:C52"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created 2 SWB figures of Myanmar
</commit_message>
<xml_diff>
--- a/Myanmar Project_Code Book.xlsx
+++ b/Myanmar Project_Code Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phyllislun/Documents/GitHub/myanmar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C17E648-3CF0-074E-93AD-745C7E8E4400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A38D9F1-3FD2-A74D-B4C8-81269F5833D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35300" yWindow="-360" windowWidth="28500" windowHeight="18380" xr2:uid="{38EF2D11-A97C-5F49-8E7A-12D4A1CCF98A}"/>
+    <workbookView xWindow="10300" yWindow="740" windowWidth="18380" windowHeight="18380" xr2:uid="{38EF2D11-A97C-5F49-8E7A-12D4A1CCF98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="172">
   <si>
     <t>Category</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>freedom of media</t>
+  </si>
+  <si>
+    <t>RESPONSE OPTIONS
+A rural area or on a farm* A small town or village* A large city* (DK)* (Refused)* A suburb of a large city*
+RESPONSE VALUES
+1* 2* 3* 4* 5* 6*</t>
+  </si>
+  <si>
+    <t>0,1</t>
   </si>
 </sst>
 </file>
@@ -712,7 +721,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1056,8 +1085,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,7 +1094,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="77.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="81.33203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
@@ -1340,6 +1369,9 @@
       <c r="F15" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G15" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1360,6 +1392,9 @@
       <c r="F16" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="G16" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1380,6 +1415,9 @@
       <c r="F17" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G17" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1400,6 +1438,9 @@
       <c r="F18" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G18" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1420,6 +1461,9 @@
       <c r="F19" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G19" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="20" spans="1:7" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
@@ -1440,6 +1484,9 @@
       <c r="F20" s="14" t="s">
         <v>126</v>
       </c>
+      <c r="G20" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1460,6 +1507,9 @@
       <c r="F21" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="G21" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1551,6 +1601,9 @@
       <c r="F26" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="G26" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1571,6 +1624,9 @@
       <c r="F27" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="G27" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1591,7 +1647,9 @@
       <c r="F28" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G28"/>
+      <c r="G28" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1612,6 +1670,9 @@
       <c r="F29" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G29" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1632,6 +1693,9 @@
       <c r="F30" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G30" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1652,8 +1716,11 @@
       <c r="F31" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1669,6 +1736,9 @@
       <c r="E32" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="F32" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1689,7 +1759,9 @@
       <c r="F33" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G33"/>
+      <c r="G33" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="34" spans="1:7" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1710,6 +1782,9 @@
       <c r="F34" s="10" t="s">
         <v>126</v>
       </c>
+      <c r="G34" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1730,7 +1805,9 @@
       <c r="F35" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="G35" s="9"/>
+      <c r="G35" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="36" spans="1:7" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1846,6 +1923,9 @@
       <c r="F41" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G41" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1866,6 +1946,9 @@
       <c r="F42" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="G42" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1886,6 +1969,9 @@
       <c r="F43" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G43" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1906,6 +1992,9 @@
       <c r="F44" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1926,6 +2015,9 @@
       <c r="F45" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G45" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="46" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1946,6 +2038,9 @@
       <c r="F46" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G46" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -1966,6 +2061,9 @@
       <c r="F47" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="G47" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -1986,8 +2084,11 @@
       <c r="F48" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -2006,8 +2107,11 @@
       <c r="F49" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -2024,7 +2128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -2041,7 +2145,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -2070,8 +2174,11 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="satisfied">
+      <formula>NOT(ISERROR(SEARCH("satisfied",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
descriptive figures of GWP data and ACLED
</commit_message>
<xml_diff>
--- a/Myanmar Project_Code Book.xlsx
+++ b/Myanmar Project_Code Book.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phyllislun/Documents/GitHub/myanmar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A38D9F1-3FD2-A74D-B4C8-81269F5833D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1D7DA8-CB27-794F-8453-8B904DFF9AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10300" yWindow="740" windowWidth="18380" windowHeight="18380" xr2:uid="{38EF2D11-A97C-5F49-8E7A-12D4A1CCF98A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="13480" windowHeight="18380" activeTab="1" xr2:uid="{38EF2D11-A97C-5F49-8E7A-12D4A1CCF98A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ACLED" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$52</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="201">
   <si>
     <t>Category</t>
   </si>
@@ -616,6 +617,93 @@
   </si>
   <si>
     <t>0,1</t>
+  </si>
+  <si>
+    <t>ACLED</t>
+  </si>
+  <si>
+    <t>event_id_cnty</t>
+  </si>
+  <si>
+    <t>A unique alphanumeric event identifier by number and country acronym. This identifier remains constant even when the event details are updated.</t>
+  </si>
+  <si>
+    <t>event_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The date on which the event took place. Recorded as Year-Month-Day.</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>The year in which the event took place.</t>
+  </si>
+  <si>
+    <t>disorder_type</t>
+  </si>
+  <si>
+    <t>The disorder category an event belongs to.</t>
+  </si>
+  <si>
+    <t>event_type</t>
+  </si>
+  <si>
+    <t>The type of event; further specifies the nature of the event.</t>
+  </si>
+  <si>
+    <t>actor1</t>
+  </si>
+  <si>
+    <t>actor2</t>
+  </si>
+  <si>
+    <t>One of two main actors involved in the event (does not necessarily indicate the aggressor).</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>A unique three-digit numeric code assigned to each country or territory according to ISO 3166.</t>
+  </si>
+  <si>
+    <t>Myanmar is 104</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>The country or territory in which the event took place.</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>admin2</t>
+  </si>
+  <si>
+    <t>admin3</t>
+  </si>
+  <si>
+    <t>The largest sub-national administrative region in which the event took place.</t>
+  </si>
+  <si>
+    <t>The second largest sub-national administrative region in which the event took place.</t>
+  </si>
+  <si>
+    <t>The third largest sub-national administrative region in which the event took place.</t>
+  </si>
+  <si>
+    <t>The name of the location at which the event took place.</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>fatalities</t>
+  </si>
+  <si>
+    <t>The number of reported fatalities arising from an event. When there are conflicting reports, the most conservative estimate is recorded.</t>
   </si>
 </sst>
 </file>
@@ -687,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -712,16 +800,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -749,6 +832,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1085,8 +1178,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,23 +1558,23 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="12" t="s">
+    <row r="20" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="4" t="s">
         <v>126</v>
       </c>
       <c r="G20" t="s">
@@ -2174,11 +2267,221 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="satisfied">
+      <formula>NOT(ISERROR(SEARCH("satisfied",F1)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F1)))</formula>
     </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92A5539-1D73-544A-88D1-C75A6BAEF899}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="73.33203125" style="1" customWidth="1"/>
+    <col min="5" max="9" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F1">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="satisfied">
       <formula>NOT(ISERROR(SEARCH("satisfied",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>